<commit_message>
Arregle un poco el formato de las tablas y agregue la variable 'partido lider'
</commit_message>
<xml_diff>
--- a/formato_tablas.xlsx
+++ b/formato_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\profesional\personal_projects\polRD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038E35A0-70FF-4D66-B82E-DDA0C7904814}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69170A0-334F-4E66-9AA2-C1921EC1798E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{4B4A90A2-7B00-4905-8F7F-B400F1541927}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>Ano</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Provincia</t>
   </si>
   <si>
-    <t>Numero de votos</t>
-  </si>
-  <si>
     <t>san jose de las matas</t>
   </si>
   <si>
@@ -115,19 +112,25 @@
     <t>vuelta</t>
   </si>
   <si>
-    <t>cantidad de colegios</t>
-  </si>
-  <si>
-    <t>cantidad inscritos</t>
-  </si>
-  <si>
     <t>votos validos</t>
   </si>
   <si>
     <t>votos nulos</t>
   </si>
   <si>
-    <t>Validos solamente desde 1998</t>
+    <t>Partido Lider</t>
+  </si>
+  <si>
+    <t>Valido solo desde 1998</t>
+  </si>
+  <si>
+    <t># de votos</t>
+  </si>
+  <si>
+    <t># de colegios</t>
+  </si>
+  <si>
+    <t># inscritos</t>
   </si>
 </sst>
 </file>
@@ -489,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BA4275-9AA4-48B6-ADAB-29DF3EF9F689}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:S5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -563,18 +564,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E123A7B-912B-4CD3-92A4-A5EB5D9A06C9}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,204 +594,225 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>25</v>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2020</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4">
         <v>1000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2024</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2024</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6">
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7">
         <v>1000</v>
       </c>
     </row>

</xml_diff>